<commit_message>
Removed all begin/end borrowed comments. Each instance was three lines showing how to access and iterator through Excel file using API.
</commit_message>
<xml_diff>
--- a/GradesCalculator/DB/GradesDatabase6300-grades.xlsx
+++ b/GradesCalculator/DB/GradesDatabase6300-grades.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Team 1</t>
   </si>
@@ -62,19 +62,12 @@
   <si>
     <t>GTID</t>
   </si>
-  <si>
-    <t>Project 4</t>
-  </si>
-  <si>
-    <t>Project 5</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -625,8 +618,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.83203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
@@ -784,10 +777,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
@@ -1050,9 +1043,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
@@ -1067,12 +1060,6 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" customHeight="1">
@@ -1320,11 +1307,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="6" width="15.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="6" width="13.1640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="6" width="13.5" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="6" width="12.6640625" collapsed="true"/>
-    <col min="5" max="16384" style="6" width="9.1640625" collapsed="true"/>
+    <col min="1" max="1" width="15.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" customHeight="1">
@@ -1339,12 +1326,6 @@
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" customHeight="1">

</xml_diff>